<commit_message>
UI Changes, other misc changes
</commit_message>
<xml_diff>
--- a/Planning/Continent.xlsx
+++ b/Planning/Continent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Desktop\Comitatus\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\GitHub\Comitatus\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BA783C-5E4B-45E3-95A2-5ECA8EAB8168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F228C4-2BAB-4E04-8C43-44688E4CDE6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A33F264D-6602-47C2-8690-3A0D3C9F96C5}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="282">
   <si>
     <t>Flat</t>
   </si>
@@ -876,6 +878,9 @@
   </si>
   <si>
     <t>Sea</t>
+  </si>
+  <si>
+    <t>Terrain Types</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF36510-DF95-4D87-8F0E-5E47258F315A}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,452 +1360,487 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>30</v>
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>39</v>
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" t="s">
+        <v>272</v>
+      </c>
+      <c r="F31" t="s">
+        <v>272</v>
+      </c>
+      <c r="G31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" t="s">
+        <v>272</v>
+      </c>
+      <c r="F32" t="s">
+        <v>272</v>
+      </c>
+      <c r="G32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" t="s">
+        <v>273</v>
+      </c>
+      <c r="F33" t="s">
+        <v>272</v>
+      </c>
+      <c r="G33" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="A34" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D34" t="s">
+        <v>273</v>
+      </c>
+      <c r="E34" t="s">
+        <v>272</v>
+      </c>
+      <c r="F34" t="s">
+        <v>272</v>
+      </c>
+      <c r="G34" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>270</v>
+        <v>277</v>
+      </c>
+      <c r="B35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" t="s">
+        <v>273</v>
+      </c>
+      <c r="F35" t="s">
+        <v>272</v>
+      </c>
+      <c r="G35" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C36" t="s">
         <v>273</v>
       </c>
       <c r="D36" t="s">
+        <v>273</v>
+      </c>
+      <c r="E36" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" t="s">
+        <v>273</v>
+      </c>
+      <c r="G36" t="s">
         <v>272</v>
-      </c>
-      <c r="E36" t="s">
-        <v>272</v>
-      </c>
-      <c r="F36" t="s">
-        <v>272</v>
-      </c>
-      <c r="G36" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B37" t="s">
-        <v>272</v>
-      </c>
-      <c r="C37" t="s">
-        <v>273</v>
-      </c>
-      <c r="D37" t="s">
-        <v>272</v>
-      </c>
-      <c r="E37" t="s">
-        <v>272</v>
-      </c>
-      <c r="F37" t="s">
-        <v>272</v>
-      </c>
-      <c r="G37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B38" t="s">
-        <v>272</v>
-      </c>
-      <c r="C38" t="s">
-        <v>273</v>
-      </c>
-      <c r="D38" t="s">
-        <v>272</v>
-      </c>
-      <c r="E38" t="s">
-        <v>273</v>
-      </c>
-      <c r="F38" t="s">
-        <v>272</v>
-      </c>
-      <c r="G38" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B39" t="s">
-        <v>272</v>
-      </c>
-      <c r="C39" t="s">
-        <v>273</v>
-      </c>
-      <c r="D39" t="s">
-        <v>273</v>
-      </c>
-      <c r="E39" t="s">
-        <v>272</v>
-      </c>
-      <c r="F39" t="s">
-        <v>272</v>
-      </c>
-      <c r="G39" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B40" t="s">
-        <v>272</v>
-      </c>
-      <c r="C40" t="s">
-        <v>273</v>
-      </c>
-      <c r="D40" t="s">
-        <v>272</v>
-      </c>
-      <c r="E40" t="s">
-        <v>273</v>
-      </c>
-      <c r="F40" t="s">
-        <v>272</v>
-      </c>
-      <c r="G40" t="s">
-        <v>273</v>
+      <c r="A40" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B41" t="s">
-        <v>273</v>
-      </c>
-      <c r="C41" t="s">
-        <v>273</v>
-      </c>
-      <c r="D41" t="s">
-        <v>273</v>
-      </c>
-      <c r="E41" t="s">
-        <v>273</v>
-      </c>
-      <c r="F41" t="s">
-        <v>273</v>
-      </c>
-      <c r="G41" t="s">
-        <v>272</v>
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O12:O24">
-    <sortCondition ref="O12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O10:O19">
+    <sortCondition ref="O10"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1812,7 +1852,7 @@
   <dimension ref="A2:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>